<commit_message>
Added histograms and updated BOM.
</commit_message>
<xml_diff>
--- a/LidarTotalBOM.xlsx
+++ b/LidarTotalBOM.xlsx
@@ -84,9 +84,6 @@
     <t>https://aliexpress.ru/item/1298052194.html</t>
   </si>
   <si>
-    <t>Original Avalanche photodiode (particly proved), 3-LCC package</t>
-  </si>
-  <si>
     <t>Chinese Avalanche photodiode (proved in real device), TO-52 package. Original photodiode costs $180 at Mouser</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>DLDC driver module based at DRV11873</t>
   </si>
   <si>
-    <t>_2_</t>
-  </si>
-  <si>
     <t>Interference Filter</t>
   </si>
   <si>
@@ -211,6 +205,12 @@
   </si>
   <si>
     <t>Optional Interference Filter,  905 +-10nm</t>
+  </si>
+  <si>
+    <t>_1_</t>
+  </si>
+  <si>
+    <t>Original Avalanche photodiode (proved), 3-LCC package</t>
   </si>
 </sst>
 </file>
@@ -291,14 +291,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,7 +625,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>8</v>
@@ -635,7 +635,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -648,14 +648,14 @@
         <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="1">
         <v>2</v>
       </c>
@@ -669,11 +669,11 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="1">
         <v>3</v>
       </c>
@@ -687,36 +687,36 @@
         <v>11</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="1"/>
       <c r="F5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="1">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D6" s="8">
         <v>9.4</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -730,11 +730,11 @@
         <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -748,11 +748,11 @@
         <v>14</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -766,11 +766,11 @@
         <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="3">
         <v>8</v>
       </c>
@@ -784,11 +784,11 @@
         <v>17</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="3">
         <v>9</v>
       </c>
@@ -800,21 +800,21 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="3">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="8">
         <v>13</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -822,16 +822,16 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="8">
         <v>9</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -839,16 +839,16 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="8">
         <v>2</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -856,16 +856,16 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="8">
         <v>2</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -873,16 +873,16 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="8">
         <v>3</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
@@ -890,16 +890,16 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D17" s="8">
         <v>12</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
@@ -907,30 +907,30 @@
         <f>SUM(D2:D17)</f>
         <v>98.4</v>
       </c>
-      <c r="E20" s="11" t="s">
-        <v>33</v>
+      <c r="E20" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="10" t="s">
-        <v>48</v>
+      <c r="B23" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D23" s="8">
         <v>27</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="10" t="s">
-        <v>48</v>
+      <c r="B24" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
@@ -939,7 +939,7 @@
         <v>23.65</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>20</v>
@@ -947,44 +947,44 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D25" s="8">
         <v>14.5</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D26" s="8">
         <v>8</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D27" s="8">
         <v>13</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some pictures added, some typos removed.
</commit_message>
<xml_diff>
--- a/LidarTotalBOM.xlsx
+++ b/LidarTotalBOM.xlsx
@@ -81,15 +81,9 @@
     <t>https://www.digikey.com/products/en?keywords=MTAPD-07-013</t>
   </si>
   <si>
-    <t>https://aliexpress.ru/item/1298052194.html</t>
-  </si>
-  <si>
     <t>Chinese Avalanche photodiode (proved in real device), TO-52 package. Original photodiode costs $180 at Mouser</t>
   </si>
   <si>
-    <t>https://aliexpress.ru/item/32817685030.html</t>
-  </si>
-  <si>
     <t>https://www.ebay.com/itm/5PCS-MAX3658AETA-T-IC-AMP-TRANSIMPEDANCE-8-TDFN-MAX3658-3658-MAX3658A-3658A-MAX3/192826918497</t>
   </si>
   <si>
@@ -126,24 +120,15 @@
     <t>Photodiode Lens</t>
   </si>
   <si>
-    <t>https://aliexpress.ru/item/32303375838.html</t>
-  </si>
-  <si>
     <t>CS lens holder</t>
   </si>
   <si>
-    <t>https://aliexpress.ru/item/32815023477.html</t>
-  </si>
-  <si>
     <t>Holder for CS lens</t>
   </si>
   <si>
     <t>BLDC motor</t>
   </si>
   <si>
-    <t>https://aliexpress.ru/item/4000323714513.html</t>
-  </si>
-  <si>
     <t>BLDC, outrunner, 20mm diameter, KV &gt; 200</t>
   </si>
   <si>
@@ -159,15 +144,9 @@
     <t>https://www.ebay.com/itm/Optical-Filter-905nm-band-pass-filter-895nm-915nm-Dia-11-5mm/262976990433</t>
   </si>
   <si>
-    <t>https://aliexpress.ru/item/32963619780.html</t>
-  </si>
-  <si>
     <t>Optional Interference Filter, 905 +-5nm, Free delivery</t>
   </si>
   <si>
-    <t>https://aliexpress.ru/item/32735300921.html</t>
-  </si>
-  <si>
     <t>Chinese Avalanche photodiode (NOT proved but similar to AD500-8), TO-52 package, interated interference filter</t>
   </si>
   <si>
@@ -177,9 +156,6 @@
     <t>Scanning Mirror</t>
   </si>
   <si>
-    <t>https://aliexpress.ru/item/4000246071735.html</t>
-  </si>
-  <si>
     <t>4 Layer PCB, price for 10 boards (&lt;50x50mm)</t>
   </si>
   <si>
@@ -219,27 +195,18 @@
     <t>https://ru.mouser.com/ProductDetail/Infineon-Technologies/BSZ165N04NSGATMA1</t>
   </si>
   <si>
-    <t>https://aliexpress.ru/item/33010069942.html</t>
-  </si>
-  <si>
     <t>DLDC driver DRV11873 (China, 1$)</t>
   </si>
   <si>
     <t>Laser lens</t>
   </si>
   <si>
-    <t>https://aliexpress.ru/item/32913215547.html</t>
-  </si>
-  <si>
     <t>25mm M12 F2.0 lens (Free delivery)</t>
   </si>
   <si>
     <t>Laser lens holder</t>
   </si>
   <si>
-    <t>https://aliexpress.ru/item/32953675441.html</t>
-  </si>
-  <si>
     <t>Customized shape, Alum, front surface mirror (price for 4 mirrors)</t>
   </si>
   <si>
@@ -252,10 +219,43 @@
     <t>M12 lens adapter</t>
   </si>
   <si>
-    <t>https://aliexpress.ru/item/32962439240.html</t>
-  </si>
-  <si>
     <t>Price for 2pcs</t>
+  </si>
+  <si>
+    <t>https://aliexpress.com/item/1298052194.html</t>
+  </si>
+  <si>
+    <t>https://aliexpress.com/item/32817685030.html</t>
+  </si>
+  <si>
+    <t>https://aliexpress.com/item/33010069942.html</t>
+  </si>
+  <si>
+    <t>https://aliexpress.com/item/32303375838.html</t>
+  </si>
+  <si>
+    <t>https://aliexpress.com/item/32815023477.html</t>
+  </si>
+  <si>
+    <t>https://aliexpress.com/item/4000323714513.html</t>
+  </si>
+  <si>
+    <t>https://aliexpress.com/item/4000246071735.html</t>
+  </si>
+  <si>
+    <t>https://aliexpress.com/item/32913215547.html</t>
+  </si>
+  <si>
+    <t>https://aliexpress.com/item/32953675441.html</t>
+  </si>
+  <si>
+    <t>https://aliexpress.com/item/32962439240.html</t>
+  </si>
+  <si>
+    <t>https://aliexpress.com/item/32735300921.html</t>
+  </si>
+  <si>
+    <t>https://aliexpress.com/item/32963619780.html</t>
   </si>
 </sst>
 </file>
@@ -649,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,7 +670,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>8</v>
@@ -693,10 +693,10 @@
         <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -714,7 +714,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -732,17 +732,17 @@
         <v>11</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="1"/>
       <c r="E5" s="4" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -751,16 +751,16 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D6" s="8">
         <v>9.4</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -778,7 +778,7 @@
         <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -796,7 +796,7 @@
         <v>14</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -814,7 +814,7 @@
         <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -823,26 +823,26 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D10" s="8">
         <v>3.5</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="1"/>
       <c r="E11" s="4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -860,7 +860,7 @@
         <v>17</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -881,16 +881,16 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" s="8">
         <v>13</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -898,16 +898,16 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D15" s="8">
         <v>9</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -915,16 +915,16 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D16" s="8">
         <v>2</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
@@ -932,16 +932,16 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D17" s="8">
         <v>2</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
@@ -949,16 +949,16 @@
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D18" s="8">
         <v>12</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
@@ -966,16 +966,16 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D19" s="8">
         <v>3.5</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
@@ -983,16 +983,16 @@
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D20" s="8">
         <v>7</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
@@ -1000,16 +1000,16 @@
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D21" s="8">
         <v>3</v>
       </c>
       <c r="E21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
@@ -1017,16 +1017,16 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D22" s="8">
         <v>2</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
@@ -1039,29 +1039,29 @@
         <v>114.4</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="9" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D29" s="8">
         <v>27</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
         <v>19</v>
@@ -1070,7 +1070,7 @@
         <v>23.65</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>20</v>
@@ -1078,44 +1078,44 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D31" s="8">
         <v>14.5</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D32" s="8">
         <v>8</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D33" s="8">
         <v>13</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1139,8 +1139,8 @@
     <hyperlink ref="F17" r:id="rId14"/>
     <hyperlink ref="F31" r:id="rId15"/>
     <hyperlink ref="F32" r:id="rId16"/>
-    <hyperlink ref="F33" r:id="rId17"/>
-    <hyperlink ref="F29" r:id="rId18"/>
+    <hyperlink ref="F33" r:id="rId17" display="https://aliexpress.ru/item/32963619780.html"/>
+    <hyperlink ref="F29" r:id="rId18" display="https://aliexpress.ru/item/32735300921.html"/>
     <hyperlink ref="F18" r:id="rId19"/>
     <hyperlink ref="F19" r:id="rId20"/>
     <hyperlink ref="F10" r:id="rId21"/>

</xml_diff>

<commit_message>
Removed wrong IR filter from BOM.
</commit_message>
<xml_diff>
--- a/LidarTotalBOM.xlsx
+++ b/LidarTotalBOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
   <si>
     <t>No.</t>
   </si>
@@ -133,12 +133,6 @@
   </si>
   <si>
     <t>Interference Filter</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/Optical-Interference-Filter-905DF40-12-5mm-Diode-Laser/152136247655</t>
-  </si>
-  <si>
-    <t>Optional Interference Filter, 905 +-3nm</t>
   </si>
   <si>
     <t>https://www.ebay.com/itm/Optical-Filter-905nm-band-pass-filter-895nm-915nm-Dia-11-5mm/262976990433</t>
@@ -650,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,7 +693,7 @@
         <v>21</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -717,7 +711,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -742,7 +736,7 @@
       <c r="A5" s="11"/>
       <c r="B5" s="1"/>
       <c r="E5" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>22</v>
@@ -754,13 +748,13 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" s="8">
         <v>9.4</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>24</v>
@@ -826,26 +820,26 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10" s="8">
         <v>3.5</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="1"/>
       <c r="E11" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -863,7 +857,7 @@
         <v>17</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -890,7 +884,7 @@
         <v>13</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>31</v>
@@ -910,7 +904,7 @@
         <v>32</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -927,7 +921,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
@@ -944,7 +938,7 @@
         <v>37</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
@@ -952,16 +946,16 @@
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D18" s="8">
         <v>12</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
@@ -969,16 +963,16 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D19" s="8">
         <v>3.5</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
@@ -986,16 +980,16 @@
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D20" s="8">
         <v>7</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
@@ -1003,16 +997,16 @@
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D21" s="8">
         <v>3</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
@@ -1020,16 +1014,16 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D22" s="8">
         <v>2</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
@@ -1051,29 +1045,29 @@
         <v>73.900000000000006</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D30" s="8">
         <v>27</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
         <v>19</v>
@@ -1082,7 +1076,7 @@
         <v>23.65</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>20</v>
@@ -1093,10 +1087,10 @@
         <v>38</v>
       </c>
       <c r="D32" s="8">
-        <v>14.5</v>
+        <v>8</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>39</v>
@@ -1107,27 +1101,13 @@
         <v>38</v>
       </c>
       <c r="D33" s="8">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="8">
-        <v>13</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1150,19 +1130,18 @@
     <hyperlink ref="F16" r:id="rId13"/>
     <hyperlink ref="F17" r:id="rId14"/>
     <hyperlink ref="F32" r:id="rId15"/>
-    <hyperlink ref="F33" r:id="rId16"/>
-    <hyperlink ref="F34" r:id="rId17" display="https://aliexpress.ru/item/32963619780.html"/>
-    <hyperlink ref="F30" r:id="rId18" display="https://aliexpress.ru/item/32735300921.html"/>
-    <hyperlink ref="F18" r:id="rId19"/>
-    <hyperlink ref="F19" r:id="rId20"/>
-    <hyperlink ref="F10" r:id="rId21"/>
-    <hyperlink ref="F11" r:id="rId22"/>
-    <hyperlink ref="F20" r:id="rId23"/>
-    <hyperlink ref="F21" r:id="rId24"/>
-    <hyperlink ref="F22" r:id="rId25"/>
+    <hyperlink ref="F33" r:id="rId16" display="https://aliexpress.ru/item/32963619780.html"/>
+    <hyperlink ref="F30" r:id="rId17" display="https://aliexpress.ru/item/32735300921.html"/>
+    <hyperlink ref="F18" r:id="rId18"/>
+    <hyperlink ref="F19" r:id="rId19"/>
+    <hyperlink ref="F10" r:id="rId20"/>
+    <hyperlink ref="F11" r:id="rId21"/>
+    <hyperlink ref="F20" r:id="rId22"/>
+    <hyperlink ref="F21" r:id="rId23"/>
+    <hyperlink ref="F22" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId25"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added image, updated BOM.
</commit_message>
<xml_diff>
--- a/LidarTotalBOM.xlsx
+++ b/LidarTotalBOM.xlsx
@@ -150,9 +150,6 @@
     <t>Scanning Mirror</t>
   </si>
   <si>
-    <t>4 Layer PCB, price for 10 boards (&lt;50x50mm)</t>
-  </si>
-  <si>
     <t>ADCMP600 x 2</t>
   </si>
   <si>
@@ -201,9 +198,6 @@
     <t>Laser lens holder</t>
   </si>
   <si>
-    <t>Customized shape, Alum, front surface mirror (price for 4 mirrors)</t>
-  </si>
-  <si>
     <t>(22$ for 5 pcs)</t>
   </si>
   <si>
@@ -213,9 +207,6 @@
     <t>M12 lens adapter</t>
   </si>
   <si>
-    <t>Price for 2pcs</t>
-  </si>
-  <si>
     <t>https://aliexpress.com/item/1298052194.html</t>
   </si>
   <si>
@@ -253,6 +244,15 @@
   </si>
   <si>
     <t>PCB components including PCB, without delivery</t>
+  </si>
+  <si>
+    <t>4 Layer PCB, price for 5 boards (&lt;50x50mm)</t>
+  </si>
+  <si>
+    <t>Price for 1pcs</t>
+  </si>
+  <si>
+    <t>Customized shape, Alum, front surface mirror (12$ for 4 mirrors)</t>
   </si>
 </sst>
 </file>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,7 +693,7 @@
         <v>21</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -711,7 +711,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -736,7 +736,7 @@
       <c r="A5" s="11"/>
       <c r="B5" s="1"/>
       <c r="E5" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>22</v>
@@ -748,13 +748,13 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="8">
         <v>9.4</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>24</v>
@@ -820,26 +820,26 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="8">
         <v>3.5</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="1"/>
       <c r="E11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -857,7 +857,7 @@
         <v>17</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -881,10 +881,10 @@
         <v>30</v>
       </c>
       <c r="D14" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>31</v>
@@ -904,7 +904,7 @@
         <v>32</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -921,7 +921,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
@@ -938,7 +938,7 @@
         <v>37</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
@@ -949,13 +949,13 @@
         <v>43</v>
       </c>
       <c r="D18" s="8">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
@@ -963,16 +963,16 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" s="8">
         <v>3.5</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
@@ -980,16 +980,16 @@
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D20" s="8">
         <v>7</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
@@ -997,16 +997,16 @@
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21" s="8">
         <v>3</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
@@ -1014,16 +1014,16 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D22" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
@@ -1033,7 +1033,7 @@
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D26" s="8">
         <f>SUM(D2:D22)</f>
-        <v>114.4</v>
+        <v>93.4</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>29</v>
@@ -1042,15 +1042,15 @@
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D27" s="8">
         <f>SUM(D2:D14)</f>
-        <v>73.900000000000006</v>
+        <v>62.9</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" t="s">
         <v>42</v>
@@ -1062,12 +1062,12 @@
         <v>41</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
         <v>19</v>
@@ -1076,7 +1076,7 @@
         <v>23.65</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>20</v>
@@ -1090,7 +1090,7 @@
         <v>8</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>39</v>
@@ -1107,7 +1107,7 @@
         <v>40</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added notes about ESD.
</commit_message>
<xml_diff>
--- a/LidarTotalBOM.xlsx
+++ b/LidarTotalBOM.xlsx
@@ -243,9 +243,6 @@
     <t>17-25</t>
   </si>
   <si>
-    <t>Chinese Avalanche photodiode NOT proved. Have IR filter modification</t>
-  </si>
-  <si>
     <t>See other variants below!</t>
   </si>
   <si>
@@ -274,6 +271,9 @@
   </si>
   <si>
     <t>Original link is not working. Orig. seller is "Ruite Professional Optical Trading Co"</t>
+  </si>
+  <si>
+    <t>Chinese Avalanche photodiode NOT proved. Has IR filter modification</t>
   </si>
 </sst>
 </file>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,7 +718,7 @@
         <v>59</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -736,7 +736,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -754,14 +754,14 @@
         <v>11</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="1"/>
       <c r="E5" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>22</v>
@@ -943,13 +943,13 @@
         <v>2</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" t="s">
         <v>82</v>
-      </c>
-      <c r="G16" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -983,10 +983,10 @@
         <v>71</v>
       </c>
       <c r="F18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" t="s">
         <v>84</v>
-      </c>
-      <c r="G18" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
@@ -1088,7 +1088,7 @@
         <v>74</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>72</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>